<commit_message>
Actuall progress, singleton removal has issue
</commit_message>
<xml_diff>
--- a/tmpresults.xlsx
+++ b/tmpresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UM\Thesis\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B630BAB9-679A-4FCF-99DF-B5ABADDE4B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A620A68-FC3A-4A9D-89A7-59D28364D1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23775" windowHeight="21000" xr2:uid="{BB6C1088-C434-4251-BD15-779699D9527C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24390" windowHeight="21000" xr2:uid="{BB6C1088-C434-4251-BD15-779699D9527C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Instance number</t>
   </si>
@@ -149,10 +149,7 @@
     <t>err</t>
   </si>
   <si>
-    <t>cherry reduction at supress</t>
-  </si>
-  <si>
-    <t>takes long</t>
+    <t>singleton suppress</t>
   </si>
 </sst>
 </file>
@@ -526,7 +523,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,11 +580,11 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E31" si="1">D3-B3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,11 +618,11 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -640,11 +637,11 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -677,15 +674,12 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -719,11 +713,11 @@
         <v>11</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -757,11 +751,11 @@
         <v>13</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,11 +770,11 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,12 +788,15 @@
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>2</v>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,12 +810,15 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,11 +833,11 @@
         <v>17</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -852,11 +852,11 @@
         <v>18</v>
       </c>
       <c r="D17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -871,11 +871,11 @@
         <v>19</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -889,12 +889,15 @@
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>2</v>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,12 +930,15 @@
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D21">
-        <v>11</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>2</v>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F21" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,11 +953,11 @@
         <v>23</v>
       </c>
       <c r="D22">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -966,11 +972,11 @@
         <v>24</v>
       </c>
       <c r="D23">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,15 +990,12 @@
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F24" t="s">
-        <v>37</v>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,11 +1010,11 @@
         <v>26</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1048,14 +1051,11 @@
         <v>28</v>
       </c>
       <c r="D27">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E27">
         <f>D27-B27</f>
-        <v>4</v>
-      </c>
-      <c r="F27" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,15 +1069,12 @@
       <c r="C28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F28" t="s">
-        <v>37</v>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1092,11 +1089,11 @@
         <v>30</v>
       </c>
       <c r="D29">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,11 +1108,11 @@
         <v>31</v>
       </c>
       <c r="D30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>